<commit_message>
Add site metadata 2018
</commit_message>
<xml_diff>
--- a/data-raw/Site Metadata Git- 2018.xlsx
+++ b/data-raw/Site Metadata Git- 2018.xlsx
@@ -974,7 +974,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1071,9 @@
       <c r="J2" s="18">
         <v>43292</v>
       </c>
-      <c r="K2" s="6"/>
+      <c r="K2" s="6">
+        <v>43320</v>
+      </c>
       <c r="M2" s="20">
         <v>3</v>
       </c>
@@ -1114,7 +1116,9 @@
       <c r="J3" s="18">
         <v>43292</v>
       </c>
-      <c r="K3" s="6"/>
+      <c r="K3" s="6">
+        <v>43320</v>
+      </c>
       <c r="M3" s="20">
         <v>3</v>
       </c>
@@ -1157,7 +1161,9 @@
       <c r="J4" s="6">
         <v>43298</v>
       </c>
-      <c r="K4" s="6"/>
+      <c r="K4" s="6">
+        <v>43325</v>
+      </c>
       <c r="L4" s="6"/>
       <c r="M4" s="20">
         <v>3</v>
@@ -1201,7 +1207,9 @@
       <c r="J5" s="18">
         <v>43292</v>
       </c>
-      <c r="K5" s="6"/>
+      <c r="K5" s="6">
+        <v>43322</v>
+      </c>
       <c r="M5" s="20">
         <v>3</v>
       </c>
@@ -1244,7 +1252,9 @@
       <c r="J6" s="18">
         <v>43292</v>
       </c>
-      <c r="K6" s="6"/>
+      <c r="K6" s="6">
+        <v>43322</v>
+      </c>
       <c r="M6" s="22">
         <v>3</v>
       </c>
@@ -1287,7 +1297,9 @@
       <c r="J7" s="19">
         <v>43293</v>
       </c>
-      <c r="K7" s="14"/>
+      <c r="K7" s="14">
+        <v>43322</v>
+      </c>
       <c r="L7" s="12"/>
       <c r="M7" s="21">
         <v>3</v>
@@ -1331,7 +1343,9 @@
       <c r="J8" s="6">
         <v>43298</v>
       </c>
-      <c r="K8" s="6"/>
+      <c r="K8" s="6">
+        <v>43327</v>
+      </c>
       <c r="L8" s="8"/>
       <c r="M8" s="23">
         <v>3</v>
@@ -1375,7 +1389,9 @@
       <c r="J9" s="6">
         <v>43298</v>
       </c>
-      <c r="K9" s="6"/>
+      <c r="K9" s="6">
+        <v>43327</v>
+      </c>
       <c r="L9" s="8"/>
       <c r="M9" s="23">
         <v>3</v>
@@ -1419,7 +1435,9 @@
       <c r="J10" s="6">
         <v>43297</v>
       </c>
-      <c r="K10" s="6"/>
+      <c r="K10" s="6">
+        <v>43321</v>
+      </c>
       <c r="M10" s="23">
         <v>3</v>
       </c>
@@ -1462,7 +1480,9 @@
       <c r="J11" s="6">
         <v>43297</v>
       </c>
-      <c r="K11" s="6"/>
+      <c r="K11" s="6">
+        <v>43321</v>
+      </c>
       <c r="M11" s="23">
         <v>3</v>
       </c>
@@ -1505,7 +1525,9 @@
       <c r="J12" s="6">
         <v>43298</v>
       </c>
-      <c r="K12" s="6"/>
+      <c r="K12" s="6">
+        <v>43326</v>
+      </c>
       <c r="M12" s="23">
         <v>3</v>
       </c>
@@ -1548,7 +1570,9 @@
       <c r="J13" s="6">
         <v>43298</v>
       </c>
-      <c r="K13" s="6"/>
+      <c r="K13" s="6">
+        <v>43326</v>
+      </c>
       <c r="L13" s="6"/>
       <c r="M13" s="23">
         <v>3</v>
@@ -1592,7 +1616,9 @@
       <c r="J14" s="6">
         <v>43299</v>
       </c>
-      <c r="K14" s="6"/>
+      <c r="K14" s="6">
+        <v>43326</v>
+      </c>
       <c r="L14" s="6"/>
       <c r="M14" s="23">
         <v>3</v>
@@ -1636,7 +1662,9 @@
       <c r="J15" s="6">
         <v>43298</v>
       </c>
-      <c r="K15" s="6"/>
+      <c r="K15" s="6">
+        <v>43326</v>
+      </c>
       <c r="L15" s="6"/>
       <c r="M15" s="23">
         <v>3</v>
@@ -1680,7 +1708,9 @@
       <c r="J16" s="6">
         <v>43298</v>
       </c>
-      <c r="K16" s="6"/>
+      <c r="K16" s="6">
+        <v>43326</v>
+      </c>
       <c r="M16" s="23">
         <v>3</v>
       </c>
@@ -1723,7 +1753,9 @@
       <c r="J17" s="6">
         <v>43298</v>
       </c>
-      <c r="K17" s="6"/>
+      <c r="K17" s="6">
+        <v>43326</v>
+      </c>
       <c r="M17" s="23">
         <v>3</v>
       </c>
@@ -1766,7 +1798,9 @@
       <c r="J18" s="6">
         <v>43298</v>
       </c>
-      <c r="K18" s="6"/>
+      <c r="K18" s="6">
+        <v>43326</v>
+      </c>
       <c r="M18" s="23">
         <v>3</v>
       </c>
@@ -1809,7 +1843,9 @@
       <c r="J19" s="18">
         <v>43293</v>
       </c>
-      <c r="K19" s="6"/>
+      <c r="K19" s="6">
+        <v>43322</v>
+      </c>
       <c r="M19" s="23">
         <v>3</v>
       </c>
@@ -1852,7 +1888,9 @@
       <c r="J20" s="18">
         <v>43293</v>
       </c>
-      <c r="K20" s="6"/>
+      <c r="K20" s="6">
+        <v>43322</v>
+      </c>
       <c r="M20" s="23">
         <v>3</v>
       </c>
@@ -1895,7 +1933,9 @@
       <c r="J21" s="6">
         <v>43297</v>
       </c>
-      <c r="K21" s="6"/>
+      <c r="K21" s="6">
+        <v>43321</v>
+      </c>
       <c r="M21" s="23">
         <v>3</v>
       </c>
@@ -1938,7 +1978,9 @@
       <c r="J22" s="6">
         <v>43297</v>
       </c>
-      <c r="K22" s="6"/>
+      <c r="K22" s="6">
+        <v>43321</v>
+      </c>
       <c r="M22" s="23">
         <v>3</v>
       </c>
@@ -1981,7 +2023,9 @@
       <c r="J23" s="6">
         <v>43297</v>
       </c>
-      <c r="K23" s="6"/>
+      <c r="K23" s="6">
+        <v>43322</v>
+      </c>
       <c r="M23" s="23">
         <v>3</v>
       </c>
@@ -2024,7 +2068,9 @@
       <c r="J24" s="6">
         <v>43298</v>
       </c>
-      <c r="K24" s="6"/>
+      <c r="K24" s="6">
+        <v>43327</v>
+      </c>
       <c r="M24" s="23">
         <v>3</v>
       </c>
@@ -2068,7 +2114,9 @@
       <c r="J25" s="6">
         <v>43298</v>
       </c>
-      <c r="K25" s="6"/>
+      <c r="K25" s="6">
+        <v>43327</v>
+      </c>
       <c r="L25" s="16"/>
       <c r="M25" s="23">
         <v>3</v>
@@ -2125,7 +2173,9 @@
       <c r="J26" s="6">
         <v>43298</v>
       </c>
-      <c r="K26" s="6"/>
+      <c r="K26" s="6">
+        <v>43327</v>
+      </c>
       <c r="M26" s="23">
         <v>3</v>
       </c>
@@ -2168,7 +2218,9 @@
       <c r="J27" s="6">
         <v>43298</v>
       </c>
-      <c r="K27" s="6"/>
+      <c r="K27" s="6">
+        <v>43327</v>
+      </c>
       <c r="M27" s="23">
         <v>3</v>
       </c>
@@ -2211,7 +2263,9 @@
       <c r="J28" s="14">
         <v>43299</v>
       </c>
-      <c r="K28" s="14"/>
+      <c r="K28" s="14">
+        <v>43326</v>
+      </c>
       <c r="L28" s="12"/>
       <c r="M28" s="21">
         <v>3</v>
@@ -2255,7 +2309,9 @@
       <c r="J29" s="18">
         <v>43292</v>
       </c>
-      <c r="K29" s="6"/>
+      <c r="K29" s="6">
+        <v>43320</v>
+      </c>
       <c r="L29" s="6"/>
       <c r="M29" s="20">
         <v>3</v>
@@ -2299,7 +2355,9 @@
       <c r="J30" s="18">
         <v>43292</v>
       </c>
-      <c r="K30" s="6"/>
+      <c r="K30" s="6">
+        <v>43320</v>
+      </c>
       <c r="M30" s="20">
         <v>3</v>
       </c>
@@ -2342,7 +2400,9 @@
       <c r="J31" s="18">
         <v>43292</v>
       </c>
-      <c r="K31" s="6"/>
+      <c r="K31" s="6">
+        <v>43320</v>
+      </c>
       <c r="M31" s="20">
         <v>3</v>
       </c>
@@ -2385,7 +2445,9 @@
       <c r="J32" s="18">
         <v>43292</v>
       </c>
-      <c r="K32" s="6"/>
+      <c r="K32" s="6">
+        <v>43320</v>
+      </c>
       <c r="L32" s="6"/>
       <c r="M32" s="20">
         <v>3</v>
@@ -2467,7 +2529,9 @@
       <c r="J34" s="18">
         <v>43292</v>
       </c>
-      <c r="K34" s="6"/>
+      <c r="K34" s="6">
+        <v>43320</v>
+      </c>
       <c r="L34" s="6"/>
       <c r="M34" s="20">
         <v>3</v>
@@ -2511,7 +2575,9 @@
       <c r="J35" s="19">
         <v>43292</v>
       </c>
-      <c r="K35" s="14"/>
+      <c r="K35" s="14">
+        <v>43320</v>
+      </c>
       <c r="L35" s="14"/>
       <c r="M35" s="21">
         <v>3</v>
@@ -2555,7 +2621,9 @@
       <c r="J36" s="6">
         <v>43297</v>
       </c>
-      <c r="K36" s="6"/>
+      <c r="K36" s="6">
+        <v>43325</v>
+      </c>
       <c r="L36" s="8"/>
       <c r="M36" s="20">
         <v>3</v>
@@ -2599,7 +2667,9 @@
       <c r="J37" s="6">
         <v>43297</v>
       </c>
-      <c r="K37" s="6"/>
+      <c r="K37" s="6">
+        <v>43325</v>
+      </c>
       <c r="L37" s="8"/>
       <c r="M37" s="20">
         <v>3</v>
@@ -2643,7 +2713,9 @@
       <c r="J38" s="6">
         <v>43297</v>
       </c>
-      <c r="K38" s="6"/>
+      <c r="K38" s="6">
+        <v>43325</v>
+      </c>
       <c r="L38" s="8"/>
       <c r="M38" s="20">
         <v>3</v>
@@ -2687,7 +2759,9 @@
       <c r="J39" s="6">
         <v>43297</v>
       </c>
-      <c r="K39" s="6"/>
+      <c r="K39" s="6">
+        <v>43325</v>
+      </c>
       <c r="M39" s="20">
         <v>3</v>
       </c>
@@ -2730,7 +2804,9 @@
       <c r="J40" s="6">
         <v>43297</v>
       </c>
-      <c r="K40" s="6"/>
+      <c r="K40" s="6">
+        <v>43325</v>
+      </c>
       <c r="L40" s="8"/>
       <c r="M40" s="20">
         <v>3</v>
@@ -2774,7 +2850,9 @@
       <c r="J41" s="6">
         <v>43297</v>
       </c>
-      <c r="K41" s="6"/>
+      <c r="K41" s="6">
+        <v>43325</v>
+      </c>
       <c r="M41" s="20">
         <v>3</v>
       </c>
@@ -2817,7 +2895,9 @@
       <c r="J42" s="6">
         <v>43297</v>
       </c>
-      <c r="K42" s="6"/>
+      <c r="K42" s="6">
+        <v>43325</v>
+      </c>
       <c r="M42" s="20">
         <v>3</v>
       </c>
@@ -2860,7 +2940,9 @@
       <c r="J43" s="6">
         <v>43297</v>
       </c>
-      <c r="K43" s="6"/>
+      <c r="K43" s="6">
+        <v>43325</v>
+      </c>
       <c r="M43" s="20">
         <v>3</v>
       </c>
@@ -2903,7 +2985,9 @@
       <c r="J44" s="6">
         <v>43297</v>
       </c>
-      <c r="K44" s="6"/>
+      <c r="K44" s="6">
+        <v>43322</v>
+      </c>
       <c r="M44" s="20">
         <v>3</v>
       </c>
@@ -2946,7 +3030,9 @@
       <c r="J45" s="6">
         <v>43297</v>
       </c>
-      <c r="K45" s="6"/>
+      <c r="K45" s="6">
+        <v>43322</v>
+      </c>
       <c r="M45" s="20">
         <v>3</v>
       </c>
@@ -2989,7 +3075,9 @@
       <c r="J46" s="18">
         <v>43293</v>
       </c>
-      <c r="K46" s="6"/>
+      <c r="K46" s="6">
+        <v>43322</v>
+      </c>
       <c r="M46" s="20">
         <v>3</v>
       </c>
@@ -3032,7 +3120,9 @@
       <c r="J47" s="6">
         <v>43298</v>
       </c>
-      <c r="K47" s="6"/>
+      <c r="K47" s="6">
+        <v>43325</v>
+      </c>
       <c r="M47" s="20">
         <v>3</v>
       </c>

</xml_diff>